<commit_message>
DataProvider used for Pim
</commit_message>
<xml_diff>
--- a/src/main/resources/excelData/OrangeHRM.xlsx
+++ b/src/main/resources/excelData/OrangeHRM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15360" windowHeight="7650"/>
+    <workbookView windowWidth="4980" windowHeight="2565" firstSheet="2" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:B5"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>UserName</t>
   </si>
@@ -46,6 +47,105 @@
   </si>
   <si>
     <t>test@4</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>SupName</t>
+  </si>
+  <si>
+    <t>MiddleNm</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>reportname</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Virat</t>
+  </si>
+  <si>
+    <t>Kohli</t>
+  </si>
+  <si>
+    <t>ronl</t>
+  </si>
+  <si>
+    <t>kohli</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF38455D"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>PIM Sample Report</t>
+    </r>
+  </si>
+  <si>
+    <t>ronaldo</t>
+  </si>
+  <si>
+    <t>Messi</t>
+  </si>
+  <si>
+    <t>mosdo</t>
+  </si>
+  <si>
+    <t>sinfho</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF38455D"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Employee Contact info report</t>
+    </r>
+  </si>
+  <si>
+    <t>rohit</t>
+  </si>
+  <si>
+    <t>mohan</t>
+  </si>
+  <si>
+    <t>sdiod</t>
+  </si>
+  <si>
+    <t>rathore</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF38455D"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>All Employee Sub Unit Hierarchy Report</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -58,13 +158,19 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF38455D"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -529,139 +635,143 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1012,8 +1122,8 @@
   <sheetPr/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1031,7 +1141,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1071,14 +1181,125 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="7"/>
+  <cols>
+    <col min="3" max="3" width="10.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="10.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="11.1428571428571" customWidth="1"/>
+    <col min="8" max="8" width="34.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>249</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>389</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>324</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>